<commit_message>
Core : create dashboard page, Minor : change icon and fixing responsivity, change password mechanism
</commit_message>
<xml_diff>
--- a/public/excel/exampleEmployee.xlsx
+++ b/public/excel/exampleEmployee.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">session_id</t>
   </si>
@@ -31,9 +31,6 @@
     <t xml:space="preserve">email</t>
   </si>
   <si>
-    <t xml:space="preserve">password</t>
-  </si>
-  <si>
     <t xml:space="preserve">nip</t>
   </si>
   <si>
@@ -44,9 +41,6 @@
   </si>
   <si>
     <t xml:space="preserve">agrasia@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">employee123</t>
   </si>
   <si>
     <t xml:space="preserve">programming</t>
@@ -93,6 +87,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -167,16 +162,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -195,28 +190,22 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="0" t="n">
+        <v>2424583749238290</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>2424583749238290</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>